<commit_message>
mRNA worst/best correl gene tables
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis_miRNA/Final Tables miRNA.xlsx
+++ b/gene_ontology_analysis_miRNA/Final Tables miRNA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporalHiC/gene_ontology_analysis_miRNA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97B4C9A-5AF2-6D4E-A72B-38DD150565DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB28DC75-36C3-CF4F-86DF-44BE044C61EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21100" yWindow="7720" windowWidth="29980" windowHeight="16100" xr2:uid="{C713BDBF-00BA-DF41-8333-6DB46E39CD97}"/>
+    <workbookView xWindow="5600" yWindow="5880" windowWidth="29980" windowHeight="16100" xr2:uid="{C713BDBF-00BA-DF41-8333-6DB46E39CD97}"/>
   </bookViews>
   <sheets>
     <sheet name="Best-Worst Correl" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="68">
   <si>
     <t>Gene</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Responsiveness to External Stimuli: Worst correlated genes often respond dynamically to external stimuli (inflammation, tissue remodeling), while best correlated genes maintain consistent expression despite environmental changes.</t>
+  </si>
+  <si>
+    <t>ß</t>
   </si>
 </sst>
 </file>
@@ -693,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AEB0E6A-EB32-1C4B-9652-0EA4D83FBA6F}">
   <dimension ref="C5:Q13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G8" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G10" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +743,7 @@
         <v>5</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>1</v>

</xml_diff>